<commit_message>
new version of the parental relationship types controlled vocabulary where some items have been depracted. See related owl:versionInfo property and readme for more information about the changes
</commit_message>
<xml_diff>
--- a/VocabolariControllati/classifications-for-people/parental-relationship-types/parental-relationship-types.xlsx
+++ b/VocabolariControllati/classifications-for-people/parental-relationship-types/parental-relationship-types.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giorgialodi/Desktop/AGID/NuovoDATIGOV/DAF/Git/OntologieVocabolariControllati/VocabolariControllati/classifications-for-people/parental-relationships/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giorgialodi/Dropbox/OntoPiA/GitOntoPiA/daf-ontologie-vocabolari-controllati/VocabolariControllati/classifications-for-people/parental-relationship-types/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E7939D9-339C-3844-B8C4-C8792B444A78}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{410D82D1-CF08-844C-911D-086F0EA9221F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9160" yWindow="460" windowWidth="18640" windowHeight="10720" xr2:uid="{7115E76C-96FC-7645-A564-32EFC4745075}"/>
+    <workbookView xWindow="6960" yWindow="460" windowWidth="18640" windowHeight="10720" xr2:uid="{7115E76C-96FC-7645-A564-32EFC4745075}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,16 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
-  <si>
-    <t>Codice_1_livello</t>
-  </si>
-  <si>
-    <t>Label_ITA_1_livello</t>
-  </si>
-  <si>
-    <t>Intestatario Scheda</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
   <si>
     <t>Marito / Moglie</t>
   </si>
@@ -68,9 +59,6 @@
     <t>Nipote (collaterale)</t>
   </si>
   <si>
-    <t>Zio / Zia (Collaterale)</t>
-  </si>
-  <si>
     <t>Cugino / Cugina</t>
   </si>
   <si>
@@ -95,12 +83,6 @@
     <t>Fratellastro / Sorellastra</t>
   </si>
   <si>
-    <t>Nipote (Affine)</t>
-  </si>
-  <si>
-    <t>Zio / Zia (Affine)</t>
-  </si>
-  <si>
     <t>Altro Affine</t>
   </si>
   <si>
@@ -126,6 +108,30 @@
   </si>
   <si>
     <t>Non definito/comunicato</t>
+  </si>
+  <si>
+    <t>codice_1_livello</t>
+  </si>
+  <si>
+    <t>label_1_livello_it</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>Non Valido</t>
+  </si>
+  <si>
+    <t>Intestatario della Scheda</t>
+  </si>
+  <si>
+    <t>Zio / Zia (collaterale)</t>
+  </si>
+  <si>
+    <t>Nipote (affine)</t>
+  </si>
+  <si>
+    <t>Zio / Zia (affine)</t>
   </si>
 </sst>
 </file>
@@ -169,10 +175,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -487,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C767BAE-CE45-EA45-B6AA-3E8A995F9070}">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -499,252 +504,276 @@
     <col min="2" max="2" width="42" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="C15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="C16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+      <c r="C20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+      <c r="C27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>80</v>
       </c>
       <c r="B29" t="s">
+        <v>23</v>
+      </c>
+      <c r="C29" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>81</v>
       </c>
       <c r="B30" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+      <c r="C30" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>99</v>
       </c>
       <c r="B31" t="s">
-        <v>31</v>
+        <v>25</v>
+      </c>
+      <c r="C31" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new version of the parental relationship types controlled vocabulary where some items have been depracted. See related owl:versionInfo property and readme for more information about the changes (#214)
Co-authored-by: Giorgia Lodi <giorgialodi@Giorgias-MBP.homenet.telecomitalia.it>
</commit_message>
<xml_diff>
--- a/VocabolariControllati/classifications-for-people/parental-relationship-types/parental-relationship-types.xlsx
+++ b/VocabolariControllati/classifications-for-people/parental-relationship-types/parental-relationship-types.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giorgialodi/Desktop/AGID/NuovoDATIGOV/DAF/Git/OntologieVocabolariControllati/VocabolariControllati/classifications-for-people/parental-relationships/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giorgialodi/Dropbox/OntoPiA/GitOntoPiA/daf-ontologie-vocabolari-controllati/VocabolariControllati/classifications-for-people/parental-relationship-types/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E7939D9-339C-3844-B8C4-C8792B444A78}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{410D82D1-CF08-844C-911D-086F0EA9221F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9160" yWindow="460" windowWidth="18640" windowHeight="10720" xr2:uid="{7115E76C-96FC-7645-A564-32EFC4745075}"/>
+    <workbookView xWindow="6960" yWindow="460" windowWidth="18640" windowHeight="10720" xr2:uid="{7115E76C-96FC-7645-A564-32EFC4745075}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,16 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
-  <si>
-    <t>Codice_1_livello</t>
-  </si>
-  <si>
-    <t>Label_ITA_1_livello</t>
-  </si>
-  <si>
-    <t>Intestatario Scheda</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
   <si>
     <t>Marito / Moglie</t>
   </si>
@@ -68,9 +59,6 @@
     <t>Nipote (collaterale)</t>
   </si>
   <si>
-    <t>Zio / Zia (Collaterale)</t>
-  </si>
-  <si>
     <t>Cugino / Cugina</t>
   </si>
   <si>
@@ -95,12 +83,6 @@
     <t>Fratellastro / Sorellastra</t>
   </si>
   <si>
-    <t>Nipote (Affine)</t>
-  </si>
-  <si>
-    <t>Zio / Zia (Affine)</t>
-  </si>
-  <si>
     <t>Altro Affine</t>
   </si>
   <si>
@@ -126,6 +108,30 @@
   </si>
   <si>
     <t>Non definito/comunicato</t>
+  </si>
+  <si>
+    <t>codice_1_livello</t>
+  </si>
+  <si>
+    <t>label_1_livello_it</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>Non Valido</t>
+  </si>
+  <si>
+    <t>Intestatario della Scheda</t>
+  </si>
+  <si>
+    <t>Zio / Zia (collaterale)</t>
+  </si>
+  <si>
+    <t>Nipote (affine)</t>
+  </si>
+  <si>
+    <t>Zio / Zia (affine)</t>
   </si>
 </sst>
 </file>
@@ -169,10 +175,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -487,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C767BAE-CE45-EA45-B6AA-3E8A995F9070}">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -499,252 +504,276 @@
     <col min="2" max="2" width="42" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="C15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="C16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+      <c r="C20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+      <c r="C27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>80</v>
       </c>
       <c r="B29" t="s">
+        <v>23</v>
+      </c>
+      <c r="C29" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>81</v>
       </c>
       <c r="B30" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+      <c r="C30" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>99</v>
       </c>
       <c r="B31" t="s">
-        <v>31</v>
+        <v>25</v>
+      </c>
+      <c r="C31" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>